<commit_message>
update with location cleaning
</commit_message>
<xml_diff>
--- a/01_input/2024_clusters_education_indicadores.xlsx
+++ b/01_input/2024_clusters_education_indicadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/paucosta_unicef_org/Documents/UNICEF/02_Cluster/02_Education/01_345w/2024_02/01_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paula.costa\Documents\GitHub\2024_ven_cluster_education_345w\01_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="688" documentId="8_{ECDDFAF1-2D4D-478B-AF6F-5BA43C0F0DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71CAFEC0-D119-4C87-91DF-DD99CC08038E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A16421-78BE-4B57-B88C-76D8D93734F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{67B5BC13-3CD3-4D4E-B40F-15C81BAB0D94}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{67B5BC13-3CD3-4D4E-B40F-15C81BAB0D94}"/>
   </bookViews>
   <sheets>
     <sheet name="educacion" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>activity</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>3.06: Distribución de kits colectivos para escuelas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.01: Implementación programas de educación y desarrollo primera infancia para NNA de 3 a 5 años dentro o fuera escuela </t>
   </si>
   <si>
     <t># de personas alcanzadas entre 12 y 17 años en escuelas o centro educativos</t>
@@ -298,6 +295,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -308,9 +308,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -328,10 +325,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -652,23 +645,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4B67F2-7701-4B0D-AA59-E0246CD6B432}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="150.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="150.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -677,290 +668,290 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="B2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>38</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
+      <c r="B6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>39</v>
+    <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>40</v>
+    <row r="11" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="12"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="12"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="12"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="12"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="12"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="12"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="12"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="4" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="12"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>41</v>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="12"/>
+      <c r="B22" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="12"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="12"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="12"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
       <c r="D25" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
       <c r="D29" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
       <c r="D30" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="7"/>
       <c r="B32" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -968,7 +959,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -976,7 +967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -984,7 +975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -992,17 +983,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1010,7 +1001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1018,7 +1009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1026,7 +1017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1034,7 +1025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1042,7 +1033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1050,17 +1041,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="7"/>
       <c r="B44" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1068,7 +1059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1076,189 +1067,194 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
+      <c r="B55" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="C55" s="6"/>
       <c r="D55" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="5" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="C37:C43"/>
-    <mergeCell ref="C44:C52"/>
-    <mergeCell ref="C53:C67"/>
-    <mergeCell ref="B53:B67"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="C26:C31"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="A44:A52"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B11:B21"/>
@@ -1271,10 +1267,21 @@
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="A11:A25"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="A44:A54"/>
     <mergeCell ref="B26:B31"/>
     <mergeCell ref="B32:B36"/>
-    <mergeCell ref="B44:B52"/>
+    <mergeCell ref="B44:B54"/>
     <mergeCell ref="B37:B43"/>
+    <mergeCell ref="A55:A69"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="C37:C43"/>
+    <mergeCell ref="C44:C54"/>
+    <mergeCell ref="C55:C69"/>
+    <mergeCell ref="B55:B69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>